<commit_message>
Update readme and add legacy code for SIFT
</commit_message>
<xml_diff>
--- a/Sensor_Fusion_Engineer/Camera/SFND_2D_Feature_Tracking-MidTermProject/PerformanceEvaluationData/PerformanceEvaluationSheet.xlsx
+++ b/Sensor_Fusion_Engineer/Camera/SFND_2D_Feature_Tracking-MidTermProject/PerformanceEvaluationData/PerformanceEvaluationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2d8bc8bef6ee2367/Nikhil_Personal/Courses/Udacity/SensorFusionEngineer/02_Camera/MidTermProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1125" documentId="11_F25DC773A252ABDACC10480A59DC4B3E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B82FB08-9B01-455A-85D2-F2B96F334CAB}"/>
+  <xr:revisionPtr revIDLastSave="1128" documentId="11_F25DC773A252ABDACC10480A59DC4B3E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0BD988B-FE4F-45DF-9F17-151918B3871F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskMP7" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="92">
   <si>
     <t>Sno</t>
   </si>
@@ -317,6 +316,9 @@
   <si>
     <t>Total Execution Time (ms)
 Detection+Description+Matching</t>
+  </si>
+  <si>
+    <t>AKAZE-AKAZE</t>
   </si>
 </sst>
 </file>
@@ -10337,7 +10339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1075C5F-C8DF-41FA-83FF-186C73325DCF}">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="C11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
@@ -11459,11 +11461,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG41"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="AG22" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="BG7" activeCellId="1" sqref="B7:B41 BG7:BG41"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12136,7 +12138,7 @@
         <v>2.7898100000000001</v>
       </c>
       <c r="BE8" s="18">
-        <f t="shared" ref="BE8:BG41" si="4">MEDIAN(AV8:BD8)</f>
+        <f t="shared" ref="BE8:BE41" si="4">MEDIAN(AV8:BD8)</f>
         <v>2.7898100000000001</v>
       </c>
       <c r="BF8" s="21">
@@ -14385,7 +14387,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="C21" s="3">
         <v>166</v>
@@ -18303,8 +18305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BEB0B4-AADC-40D3-90FA-3B723F9F987F}">
   <dimension ref="A1:B188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V166" sqref="V166"/>
+    <sheetView topLeftCell="A112" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B194" sqref="B194:B205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Update performance sheet and images
</commit_message>
<xml_diff>
--- a/Sensor_Fusion_Engineer/Camera/SFND_2D_Feature_Tracking-MidTermProject/PerformanceEvaluationData/PerformanceEvaluationSheet.xlsx
+++ b/Sensor_Fusion_Engineer/Camera/SFND_2D_Feature_Tracking-MidTermProject/PerformanceEvaluationData/PerformanceEvaluationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2d8bc8bef6ee2367/Nikhil_Personal/Courses/Udacity/SensorFusionEngineer/02_Camera/MidTermProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1128" documentId="11_F25DC773A252ABDACC10480A59DC4B3E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0BD988B-FE4F-45DF-9F17-151918B3871F}"/>
+  <xr:revisionPtr revIDLastSave="1181" documentId="11_F25DC773A252ABDACC10480A59DC4B3E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3DE1F6A-E1BC-4A28-9A49-432BF5050885}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TaskMP7" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="TaskMP8_9_Chart_Data" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TaskMP8_9_Chart_Data!$A$1:$B$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -349,7 +352,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,6 +392,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -519,7 +528,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -612,6 +621,20 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2100,654 +2123,6 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>TaskMP8_9_Chart_Data!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Median Descriptor Execution Time (ms)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>TaskMP8_9_Chart_Data!$A$2:$A$36</c:f>
-              <c:strCache>
-                <c:ptCount val="35"/>
-                <c:pt idx="0">
-                  <c:v>SIFT-SIFT</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>ORB-SIFT</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>AKAZE-FREAK</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>AKAZE-FREAK</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>SHITOMASI-FREAK</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>FAST-FREAK</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>FAST-SIFT</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>BRISK-SIFT</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>BRISK-FREAK</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>SHITOMASI-SIFT</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>HARRIS-FREAK</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>AKAZE-SIFT</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>SIFT-FREAK</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>ORB-FREAK</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>HARRIS-SIFT</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>ORB-ORB</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>BRISK-ORB</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>AKAZE-ORB</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>ORB-BRISK</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>SHITOMASI-ORB</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>HARRIS-ORB</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>FAST-ORB</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>BRISK-BRISK</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>FAST-BRISK</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>SHITOMASI-BRISK</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>SIFT-BRISK</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>ORB-BRIEF</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>FAST-BRIEF</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>AKAZE-BRISK</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>BRISK-BRIEF</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>SHITOMASI-BRIEF</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>HARRIS-BRISK</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>SIFT-BRIEF</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>HARRIS-BRIEF</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>AKAZE-BRIEF</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>TaskMP8_9_Chart_Data!$B$2:$B$36</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
-                <c:pt idx="0">
-                  <c:v>96.905299999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>96.157049999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>94.70805</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42.960949999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42.25685</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41.726150000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>36.685299999999998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>36.661200000000001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>34.132199999999997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>33.799049999999994</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>32.234400000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>31.96715</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>31.610949999999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>27.619500000000002</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>26.608450000000001</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16.752949999999998</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>15.6242</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>11.343599999999999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8.1175350000000002</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7.1380300000000005</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.8861799999999995</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4.8041850000000004</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4.5026849999999996</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>4.0987349999999996</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.7286000000000001</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.4825200000000001</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.4035099999999998</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.1448100000000001</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2.0352800000000002</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.7925249999999999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.5541800000000001</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.31429</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1.3086250000000001</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1.2672699999999999</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.0145919999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9645-49E2-92B9-5C89E63B5ABF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="115"/>
-        <c:overlap val="-20"/>
-        <c:axId val="1576485119"/>
-        <c:axId val="1576513439"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1576485119"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Detector - Descriptor</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Combination</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1576513439"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1576513439"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="5000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time (ms)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1576485119"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
               <c:f>TaskMP8_9_Chart_Data!$B$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -2872,7 +2247,7 @@
                   <c:v>AKAZE-SIFT</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>AKAZE-FREAK</c:v>
+                  <c:v>AKAZE-AKAZE</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>AKAZE-BRIEF</c:v>
@@ -3336,7 +2711,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3540,7 +2915,7 @@
                   <c:v>AKAZE-SIFT</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>AKAZE-FREAK</c:v>
+                  <c:v>AKAZE-AKAZE</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>HARRIS-BRIEF</c:v>
@@ -3933,7 +3308,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4095,7 +3470,7 @@
                   <c:v>BRISK-ORB</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>AKAZE-FREAK</c:v>
+                  <c:v>AKAZE-AKAZE</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>FAST-SIFT</c:v>
@@ -4611,7 +3986,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4731,7 +4106,7 @@
                   <c:v>SIFT-SIFT</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>AKAZE-FREAK</c:v>
+                  <c:v>AKAZE-AKAZE</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>AKAZE-FREAK</c:v>
@@ -5198,6 +4573,641 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TaskMP8_9_Chart_Data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Median Descriptor Execution Time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>TaskMP8_9_Chart_Data!$A$2:$A$36</c:f>
+              <c:strCache>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>SIFT-SIFT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ORB-SIFT</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AKAZE-AKAZE</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AKAZE-FREAK</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SHITOMASI-FREAK</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>FAST-FREAK</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>FAST-SIFT</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>BRISK-SIFT</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>BRISK-FREAK</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>SHITOMASI-SIFT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>HARRIS-FREAK</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>AKAZE-SIFT</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>SIFT-FREAK</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>ORB-FREAK</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>HARRIS-SIFT</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>ORB-ORB</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>BRISK-ORB</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>AKAZE-ORB</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>ORB-BRISK</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>SHITOMASI-ORB</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>HARRIS-ORB</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>FAST-ORB</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>BRISK-BRISK</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>FAST-BRISK</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>SHITOMASI-BRISK</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>SIFT-BRISK</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>ORB-BRIEF</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>FAST-BRIEF</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>AKAZE-BRISK</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>BRISK-BRIEF</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>SHITOMASI-BRIEF</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>HARRIS-BRISK</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>SIFT-BRIEF</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>HARRIS-BRIEF</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>AKAZE-BRIEF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TaskMP8_9_Chart_Data!$B$2:$B$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>96.905299999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96.157049999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>94.70805</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42.960949999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42.25685</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41.726150000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36.685299999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36.661200000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34.132199999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.799049999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.234400000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>31.96715</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>31.610949999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27.619500000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26.608450000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.752949999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15.6242</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11.343599999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.1175350000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.1380300000000005</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.8861799999999995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.8041850000000004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.5026849999999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.0987349999999996</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.7286000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.4825200000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.4035099999999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.1448100000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.0352800000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.7925249999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.5541800000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.31429</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.3086250000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.2672699999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.0145919999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6006-42F7-864D-8C4DD0D59903}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="115"/>
+        <c:overlap val="-20"/>
+        <c:axId val="143051487"/>
+        <c:axId val="142156799"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="143051487"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>detector -descriptor combination</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="142156799"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="142156799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="143051487"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -9890,42 +9900,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>371474</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A87A26B-BAB0-1DA5-331E-AD74F15B593D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
       <xdr:colOff>219074</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
@@ -9953,7 +9927,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9989,7 +9963,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10025,7 +9999,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10050,6 +10024,42 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5EFE6DE-4934-79F6-199E-01708FCDFE74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>64407</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>5894</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>214539</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>176891</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E201FDC-2063-3350-CF25-A6AF79036E42}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10339,7 +10349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1075C5F-C8DF-41FA-83FF-186C73325DCF}">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="C18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
@@ -11461,11 +11471,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomRight" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12150,188 +12160,188 @@
         <v>19.08297</v>
       </c>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
+    <row r="9" spans="1:59" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="33">
         <v>3</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="33">
         <v>617</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="33">
         <v>617</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="33">
         <v>614</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="33">
         <v>623</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="33">
         <v>601</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="33">
         <v>625</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="33">
         <v>610</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="33">
         <v>618</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="33">
         <v>588</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="33">
         <v>583</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="33">
         <f t="shared" si="0"/>
         <v>615.5</v>
       </c>
-      <c r="N9" s="16">
+      <c r="N9" s="34">
         <v>15.526300000000001</v>
       </c>
-      <c r="O9" s="16">
+      <c r="O9" s="34">
         <v>19.067499999999999</v>
       </c>
-      <c r="P9" s="16">
+      <c r="P9" s="34">
         <v>8.7157300000000006</v>
       </c>
-      <c r="Q9" s="16">
+      <c r="Q9" s="34">
         <v>8.3360500000000002</v>
       </c>
-      <c r="R9" s="16">
+      <c r="R9" s="34">
         <v>24.380600000000001</v>
       </c>
-      <c r="S9" s="16">
+      <c r="S9" s="34">
         <v>14.524900000000001</v>
       </c>
-      <c r="T9" s="16">
+      <c r="T9" s="34">
         <v>15.1745</v>
       </c>
-      <c r="U9" s="16">
+      <c r="U9" s="34">
         <v>8.36069</v>
       </c>
-      <c r="V9" s="16">
+      <c r="V9" s="34">
         <v>16.466899999999999</v>
       </c>
-      <c r="W9" s="16">
+      <c r="W9" s="34">
         <v>51.621899999999997</v>
       </c>
-      <c r="X9" s="18">
+      <c r="X9" s="34">
         <f t="shared" si="1"/>
         <v>15.3504</v>
       </c>
-      <c r="Y9" s="16">
+      <c r="Y9" s="34">
         <v>48.1524</v>
       </c>
-      <c r="Z9" s="16">
+      <c r="Z9" s="34">
         <v>11.9192</v>
       </c>
-      <c r="AA9" s="16">
+      <c r="AA9" s="34">
         <v>16.055900000000001</v>
       </c>
-      <c r="AB9" s="16">
+      <c r="AB9" s="34">
         <v>18.843499999999999</v>
       </c>
-      <c r="AC9" s="16">
+      <c r="AC9" s="34">
         <v>19.6005</v>
       </c>
-      <c r="AD9" s="16">
+      <c r="AD9" s="34">
         <v>16.648</v>
       </c>
-      <c r="AE9" s="16">
+      <c r="AE9" s="34">
         <v>13.925700000000001</v>
       </c>
-      <c r="AF9" s="16">
+      <c r="AF9" s="34">
         <v>17.996200000000002</v>
       </c>
-      <c r="AG9" s="16">
+      <c r="AG9" s="34">
         <v>16.7484</v>
       </c>
-      <c r="AH9" s="16">
+      <c r="AH9" s="34">
         <v>16.7575</v>
       </c>
-      <c r="AI9" s="18">
+      <c r="AI9" s="34">
         <f t="shared" si="2"/>
         <v>16.752949999999998</v>
       </c>
-      <c r="AJ9" s="3" t="e">
+      <c r="AJ9" s="33" t="e">
         <v>#N/A</v>
       </c>
-      <c r="AK9" s="3">
+      <c r="AK9" s="33">
         <v>402</v>
       </c>
-      <c r="AL9" s="3">
+      <c r="AL9" s="33">
         <v>435</v>
       </c>
-      <c r="AM9" s="3">
+      <c r="AM9" s="33">
         <v>404</v>
       </c>
-      <c r="AN9" s="3">
+      <c r="AN9" s="33">
         <v>410</v>
       </c>
-      <c r="AO9" s="3">
+      <c r="AO9" s="33">
         <v>408</v>
       </c>
-      <c r="AP9" s="3">
+      <c r="AP9" s="33">
         <v>461</v>
       </c>
-      <c r="AQ9" s="3">
+      <c r="AQ9" s="33">
         <v>415</v>
       </c>
-      <c r="AR9" s="3">
+      <c r="AR9" s="33">
         <v>417</v>
       </c>
-      <c r="AS9" s="3">
+      <c r="AS9" s="33">
         <v>430</v>
       </c>
-      <c r="AT9" s="19">
+      <c r="AT9" s="33">
         <f t="shared" si="3"/>
         <v>415</v>
       </c>
-      <c r="AU9" s="3" t="e">
+      <c r="AU9" s="33" t="e">
         <v>#N/A</v>
       </c>
-      <c r="AV9" s="16">
+      <c r="AV9" s="34">
         <v>3.29833</v>
       </c>
-      <c r="AW9" s="16">
+      <c r="AW9" s="34">
         <v>3.16228</v>
       </c>
-      <c r="AX9" s="16">
+      <c r="AX9" s="34">
         <v>3.1486299999999998</v>
       </c>
-      <c r="AY9" s="16">
+      <c r="AY9" s="34">
         <v>2.8163</v>
       </c>
-      <c r="AZ9" s="16">
+      <c r="AZ9" s="34">
         <v>3.0121500000000001</v>
       </c>
-      <c r="BA9" s="16">
+      <c r="BA9" s="34">
         <v>3.5873499999999998</v>
       </c>
-      <c r="BB9" s="16">
+      <c r="BB9" s="34">
         <v>3.9777499999999999</v>
       </c>
-      <c r="BC9" s="16">
+      <c r="BC9" s="34">
         <v>7.4453699999999996</v>
       </c>
-      <c r="BD9" s="16">
+      <c r="BD9" s="34">
         <v>3.1918799999999998</v>
       </c>
-      <c r="BE9" s="18">
+      <c r="BE9" s="34">
         <f t="shared" si="4"/>
         <v>3.1918799999999998</v>
       </c>
-      <c r="BF9" s="21">
+      <c r="BF9" s="35">
         <f t="shared" si="5"/>
         <v>0.67424857839155161</v>
       </c>
-      <c r="BG9" s="18">
+      <c r="BG9" s="34">
         <f t="shared" si="6"/>
         <v>35.295229999999997</v>
       </c>
@@ -12708,188 +12718,188 @@
         <v>116.95002000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
+    <row r="12" spans="1:59" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="33">
         <v>6</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="33">
         <v>264</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="33">
         <v>282</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="33">
         <v>282</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="33">
         <v>277</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="33">
         <v>297</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="33">
         <v>279</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="33">
         <v>289</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="33">
         <v>272</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="33">
         <v>266</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="33">
         <v>254</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="33">
         <f t="shared" si="0"/>
         <v>278</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="34">
         <v>88.227599999999995</v>
       </c>
-      <c r="O12" s="16">
+      <c r="O12" s="34">
         <v>61.016500000000001</v>
       </c>
-      <c r="P12" s="16">
+      <c r="P12" s="34">
         <v>63.0717</v>
       </c>
-      <c r="Q12" s="16">
+      <c r="Q12" s="34">
         <v>60.108899999999998</v>
       </c>
-      <c r="R12" s="16">
+      <c r="R12" s="34">
         <v>104.85599999999999</v>
       </c>
-      <c r="S12" s="16">
+      <c r="S12" s="34">
         <v>62.815100000000001</v>
       </c>
-      <c r="T12" s="16">
+      <c r="T12" s="34">
         <v>98.549899999999994</v>
       </c>
-      <c r="U12" s="16">
+      <c r="U12" s="34">
         <v>60.738700000000001</v>
       </c>
-      <c r="V12" s="16">
+      <c r="V12" s="34">
         <v>59.2879</v>
       </c>
-      <c r="W12" s="16">
+      <c r="W12" s="34">
         <v>61.237000000000002</v>
       </c>
-      <c r="X12" s="18">
+      <c r="X12" s="34">
         <f t="shared" si="1"/>
         <v>62.026049999999998</v>
       </c>
-      <c r="Y12" s="16">
+      <c r="Y12" s="34">
         <v>3.1952199999999999</v>
       </c>
-      <c r="Z12" s="16">
+      <c r="Z12" s="34">
         <v>4.5265899999999997</v>
       </c>
-      <c r="AA12" s="16">
+      <c r="AA12" s="34">
         <v>3.9824799999999998</v>
       </c>
-      <c r="AB12" s="16">
+      <c r="AB12" s="34">
         <v>4.5719200000000004</v>
       </c>
-      <c r="AC12" s="16">
+      <c r="AC12" s="34">
         <v>5.3657199999999996</v>
       </c>
-      <c r="AD12" s="16">
+      <c r="AD12" s="34">
         <v>6.4135299999999997</v>
       </c>
-      <c r="AE12" s="16">
+      <c r="AE12" s="34">
         <v>3.7928999999999999</v>
       </c>
-      <c r="AF12" s="16">
+      <c r="AF12" s="34">
         <v>4.8778800000000002</v>
       </c>
-      <c r="AG12" s="16">
+      <c r="AG12" s="34">
         <v>3.92997</v>
       </c>
-      <c r="AH12" s="16">
+      <c r="AH12" s="34">
         <v>4.4787800000000004</v>
       </c>
-      <c r="AI12" s="18">
+      <c r="AI12" s="34">
         <f t="shared" si="2"/>
         <v>4.5026849999999996</v>
       </c>
-      <c r="AJ12" s="3" t="e">
+      <c r="AJ12" s="33" t="e">
         <v>#N/A</v>
       </c>
-      <c r="AK12" s="3">
+      <c r="AK12" s="33">
         <v>171</v>
       </c>
-      <c r="AL12" s="3">
+      <c r="AL12" s="33">
         <v>176</v>
       </c>
-      <c r="AM12" s="3">
+      <c r="AM12" s="33">
         <v>157</v>
       </c>
-      <c r="AN12" s="3">
+      <c r="AN12" s="33">
         <v>176</v>
       </c>
-      <c r="AO12" s="3">
+      <c r="AO12" s="33">
         <v>174</v>
       </c>
-      <c r="AP12" s="3">
+      <c r="AP12" s="33">
         <v>188</v>
       </c>
-      <c r="AQ12" s="3">
+      <c r="AQ12" s="33">
         <v>173</v>
       </c>
-      <c r="AR12" s="3">
+      <c r="AR12" s="33">
         <v>171</v>
       </c>
-      <c r="AS12" s="3">
+      <c r="AS12" s="33">
         <v>184</v>
       </c>
-      <c r="AT12" s="19">
+      <c r="AT12" s="33">
         <f t="shared" si="3"/>
         <v>174</v>
       </c>
-      <c r="AU12" s="3" t="e">
+      <c r="AU12" s="33" t="e">
         <v>#N/A</v>
       </c>
-      <c r="AV12" s="16">
+      <c r="AV12" s="34">
         <v>0.97436299999999998</v>
       </c>
-      <c r="AW12" s="16">
+      <c r="AW12" s="34">
         <v>0.89747299999999997</v>
       </c>
-      <c r="AX12" s="16">
+      <c r="AX12" s="34">
         <v>3.2788499999999998</v>
       </c>
-      <c r="AY12" s="16">
+      <c r="AY12" s="34">
         <v>1.01576</v>
       </c>
-      <c r="AZ12" s="16">
+      <c r="AZ12" s="34">
         <v>0.89631899999999998</v>
       </c>
-      <c r="BA12" s="16">
+      <c r="BA12" s="34">
         <v>1.18963</v>
       </c>
-      <c r="BB12" s="16">
+      <c r="BB12" s="34">
         <v>1.2813399999999999</v>
       </c>
-      <c r="BC12" s="16">
+      <c r="BC12" s="34">
         <v>1.7154100000000001</v>
       </c>
-      <c r="BD12" s="16">
+      <c r="BD12" s="34">
         <v>6.6838600000000001</v>
       </c>
-      <c r="BE12" s="18">
+      <c r="BE12" s="34">
         <f t="shared" si="4"/>
         <v>1.18963</v>
       </c>
-      <c r="BF12" s="21">
+      <c r="BF12" s="35">
         <f t="shared" si="5"/>
         <v>0.62589928057553956</v>
       </c>
-      <c r="BG12" s="18">
+      <c r="BG12" s="34">
         <f t="shared" si="6"/>
         <v>67.718364999999991</v>
       </c>
@@ -14382,188 +14392,188 @@
         <v>192.62888800000002</v>
       </c>
     </row>
-    <row r="21" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
+    <row r="21" spans="1:59" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="33">
         <v>15</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="33">
         <v>166</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="33">
         <v>157</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="33">
         <v>161</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="33">
         <v>155</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="33">
         <v>163</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="33">
         <v>164</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="33">
         <v>173</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="33">
         <v>175</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21" s="33">
         <v>177</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="33">
         <v>179</v>
       </c>
-      <c r="M21" s="19">
+      <c r="M21" s="33">
         <f t="shared" si="0"/>
         <v>165</v>
       </c>
-      <c r="N21" s="16">
+      <c r="N21" s="34">
         <v>252.601</v>
       </c>
-      <c r="O21" s="16">
+      <c r="O21" s="34">
         <v>158.59100000000001</v>
       </c>
-      <c r="P21" s="16">
+      <c r="P21" s="34">
         <v>119.931</v>
       </c>
-      <c r="Q21" s="16">
+      <c r="Q21" s="34">
         <v>124.47199999999999</v>
       </c>
-      <c r="R21" s="16">
+      <c r="R21" s="34">
         <v>107.7</v>
       </c>
-      <c r="S21" s="16">
+      <c r="S21" s="34">
         <v>124.60599999999999</v>
       </c>
-      <c r="T21" s="16">
+      <c r="T21" s="34">
         <v>130.75399999999999</v>
       </c>
-      <c r="U21" s="16">
+      <c r="U21" s="34">
         <v>120.41800000000001</v>
       </c>
-      <c r="V21" s="16">
+      <c r="V21" s="34">
         <v>105.76900000000001</v>
       </c>
-      <c r="W21" s="16">
+      <c r="W21" s="34">
         <v>97.805400000000006</v>
       </c>
-      <c r="X21" s="18">
+      <c r="X21" s="34">
         <f t="shared" si="1"/>
         <v>122.44499999999999</v>
       </c>
-      <c r="Y21" s="16">
+      <c r="Y21" s="34">
         <v>163.38200000000001</v>
       </c>
-      <c r="Z21" s="16">
+      <c r="Z21" s="34">
         <v>129.85900000000001</v>
       </c>
-      <c r="AA21" s="16">
+      <c r="AA21" s="34">
         <v>83.041600000000003</v>
       </c>
-      <c r="AB21" s="16">
+      <c r="AB21" s="34">
         <v>79.715800000000002</v>
       </c>
-      <c r="AC21" s="16">
+      <c r="AC21" s="34">
         <v>161.64099999999999</v>
       </c>
-      <c r="AD21" s="16">
+      <c r="AD21" s="34">
         <v>152.44999999999999</v>
       </c>
-      <c r="AE21" s="16">
+      <c r="AE21" s="34">
         <v>90.054199999999994</v>
       </c>
-      <c r="AF21" s="16">
+      <c r="AF21" s="34">
         <v>81.021500000000003</v>
       </c>
-      <c r="AG21" s="16">
+      <c r="AG21" s="34">
         <v>92.882900000000006</v>
       </c>
-      <c r="AH21" s="16">
+      <c r="AH21" s="34">
         <v>96.533199999999994</v>
       </c>
-      <c r="AI21" s="18">
+      <c r="AI21" s="34">
         <f t="shared" si="2"/>
         <v>94.70805</v>
       </c>
-      <c r="AJ21" s="3" t="e">
+      <c r="AJ21" s="33" t="e">
         <v>#N/A</v>
       </c>
-      <c r="AK21" s="3">
+      <c r="AK21" s="33">
         <v>138</v>
       </c>
-      <c r="AL21" s="3">
+      <c r="AL21" s="33">
         <v>138</v>
       </c>
-      <c r="AM21" s="3">
+      <c r="AM21" s="33">
         <v>133</v>
       </c>
-      <c r="AN21" s="3">
+      <c r="AN21" s="33">
         <v>127</v>
       </c>
-      <c r="AO21" s="3">
+      <c r="AO21" s="33">
         <v>129</v>
       </c>
-      <c r="AP21" s="3">
+      <c r="AP21" s="33">
         <v>146</v>
       </c>
-      <c r="AQ21" s="3">
+      <c r="AQ21" s="33">
         <v>147</v>
       </c>
-      <c r="AR21" s="3">
+      <c r="AR21" s="33">
         <v>151</v>
       </c>
-      <c r="AS21" s="3">
+      <c r="AS21" s="33">
         <v>150</v>
       </c>
-      <c r="AT21" s="19">
+      <c r="AT21" s="33">
         <f t="shared" si="3"/>
         <v>138</v>
       </c>
-      <c r="AU21" s="3" t="e">
+      <c r="AU21" s="33" t="e">
         <v>#N/A</v>
       </c>
-      <c r="AV21" s="16">
+      <c r="AV21" s="34">
         <v>0.78540600000000005</v>
       </c>
-      <c r="AW21" s="16">
+      <c r="AW21" s="34">
         <v>0.67304299999999995</v>
       </c>
-      <c r="AX21" s="16">
+      <c r="AX21" s="34">
         <v>24.5044</v>
       </c>
-      <c r="AY21" s="16">
+      <c r="AY21" s="34">
         <v>0.95036600000000004</v>
       </c>
-      <c r="AZ21" s="16">
+      <c r="AZ21" s="34">
         <v>0.73463100000000003</v>
       </c>
-      <c r="BA21" s="16">
+      <c r="BA21" s="34">
         <v>0.57425400000000004</v>
       </c>
-      <c r="BB21" s="16">
+      <c r="BB21" s="34">
         <v>3.32118</v>
       </c>
-      <c r="BC21" s="16">
+      <c r="BC21" s="34">
         <v>5.08744</v>
       </c>
-      <c r="BD21" s="16">
+      <c r="BD21" s="34">
         <v>11.1198</v>
       </c>
-      <c r="BE21" s="18">
+      <c r="BE21" s="34">
         <f t="shared" si="4"/>
         <v>0.95036600000000004</v>
       </c>
-      <c r="BF21" s="21">
+      <c r="BF21" s="35">
         <f t="shared" si="5"/>
         <v>0.83636363636363631</v>
       </c>
-      <c r="BG21" s="18">
+      <c r="BG21" s="34">
         <f t="shared" si="6"/>
         <v>218.10341600000001</v>
       </c>
@@ -16242,188 +16252,188 @@
         <v>175.388091</v>
       </c>
     </row>
-    <row r="31" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A31" s="3">
+    <row r="31" spans="1:59" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="33">
         <v>25</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="33">
         <v>138</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="33">
         <v>132</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="33">
         <v>124</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="33">
         <v>137</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="33">
         <v>134</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="33">
         <v>140</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="33">
         <v>137</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="33">
         <v>148</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K31" s="33">
         <v>159</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L31" s="33">
         <v>137</v>
       </c>
-      <c r="M31" s="19">
+      <c r="M31" s="33">
         <f t="shared" si="0"/>
         <v>137</v>
       </c>
-      <c r="N31" s="16">
+      <c r="N31" s="34">
         <v>171.31700000000001</v>
       </c>
-      <c r="O31" s="16">
+      <c r="O31" s="34">
         <v>177.517</v>
       </c>
-      <c r="P31" s="16">
+      <c r="P31" s="34">
         <v>133.59</v>
       </c>
-      <c r="Q31" s="16">
+      <c r="Q31" s="34">
         <v>147.56399999999999</v>
       </c>
-      <c r="R31" s="16">
+      <c r="R31" s="34">
         <v>132.583</v>
       </c>
-      <c r="S31" s="16">
+      <c r="S31" s="34">
         <v>119.021</v>
       </c>
-      <c r="T31" s="16">
+      <c r="T31" s="34">
         <v>131.559</v>
       </c>
-      <c r="U31" s="16">
+      <c r="U31" s="34">
         <v>118.76300000000001</v>
       </c>
-      <c r="V31" s="16">
+      <c r="V31" s="34">
         <v>125.78400000000001</v>
       </c>
-      <c r="W31" s="16">
+      <c r="W31" s="34">
         <v>141.447</v>
       </c>
-      <c r="X31" s="18">
+      <c r="X31" s="34">
         <f t="shared" si="1"/>
         <v>133.0865</v>
       </c>
-      <c r="Y31" s="16">
+      <c r="Y31" s="34">
         <v>76.460700000000003</v>
       </c>
-      <c r="Z31" s="16">
+      <c r="Z31" s="34">
         <v>98.1935</v>
       </c>
-      <c r="AA31" s="16">
+      <c r="AA31" s="34">
         <v>89.497200000000007</v>
       </c>
-      <c r="AB31" s="16">
+      <c r="AB31" s="34">
         <v>100.501</v>
       </c>
-      <c r="AC31" s="16">
+      <c r="AC31" s="34">
         <v>100.431</v>
       </c>
-      <c r="AD31" s="16">
+      <c r="AD31" s="34">
         <v>87.859099999999998</v>
       </c>
-      <c r="AE31" s="16">
+      <c r="AE31" s="34">
         <v>99.882800000000003</v>
       </c>
-      <c r="AF31" s="16">
+      <c r="AF31" s="34">
         <v>90.658600000000007</v>
       </c>
-      <c r="AG31" s="16">
+      <c r="AG31" s="34">
         <v>101.578</v>
       </c>
-      <c r="AH31" s="16">
+      <c r="AH31" s="34">
         <v>95.617099999999994</v>
       </c>
-      <c r="AI31" s="18">
+      <c r="AI31" s="34">
         <f t="shared" si="2"/>
         <v>96.905299999999997</v>
       </c>
-      <c r="AJ31" s="3" t="e">
+      <c r="AJ31" s="33" t="e">
         <v>#N/A</v>
       </c>
-      <c r="AK31" s="3">
+      <c r="AK31" s="33">
         <v>82</v>
       </c>
-      <c r="AL31" s="3">
+      <c r="AL31" s="33">
         <v>81</v>
       </c>
-      <c r="AM31" s="3">
+      <c r="AM31" s="33">
         <v>85</v>
       </c>
-      <c r="AN31" s="3">
+      <c r="AN31" s="33">
         <v>93</v>
       </c>
-      <c r="AO31" s="3">
+      <c r="AO31" s="33">
         <v>90</v>
       </c>
-      <c r="AP31" s="3">
+      <c r="AP31" s="33">
         <v>81</v>
       </c>
-      <c r="AQ31" s="3">
+      <c r="AQ31" s="33">
         <v>82</v>
       </c>
-      <c r="AR31" s="3">
+      <c r="AR31" s="33">
         <v>102</v>
       </c>
-      <c r="AS31" s="3">
+      <c r="AS31" s="33">
         <v>104</v>
       </c>
-      <c r="AT31" s="19">
+      <c r="AT31" s="33">
         <f t="shared" si="3"/>
         <v>85</v>
       </c>
-      <c r="AU31" s="3" t="e">
+      <c r="AU31" s="33" t="e">
         <v>#N/A</v>
       </c>
-      <c r="AV31" s="16">
+      <c r="AV31" s="34">
         <v>0.30255700000000002</v>
       </c>
-      <c r="AW31" s="16">
+      <c r="AW31" s="34">
         <v>0.25748399999999999</v>
       </c>
-      <c r="AX31" s="16">
+      <c r="AX31" s="34">
         <v>0.22392799999999999</v>
       </c>
-      <c r="AY31" s="16">
+      <c r="AY31" s="34">
         <v>0.59863</v>
       </c>
-      <c r="AZ31" s="16">
+      <c r="AZ31" s="34">
         <v>0.59176200000000001</v>
       </c>
-      <c r="BA31" s="16">
+      <c r="BA31" s="34">
         <v>0.344725</v>
       </c>
-      <c r="BB31" s="16">
+      <c r="BB31" s="34">
         <v>0.62690800000000002</v>
       </c>
-      <c r="BC31" s="16">
+      <c r="BC31" s="34">
         <v>0.58953199999999994</v>
       </c>
-      <c r="BD31" s="16">
+      <c r="BD31" s="34">
         <v>0.35512100000000002</v>
       </c>
-      <c r="BE31" s="18">
+      <c r="BE31" s="34">
         <f t="shared" si="4"/>
         <v>0.35512100000000002</v>
       </c>
-      <c r="BF31" s="21">
+      <c r="BF31" s="35">
         <f t="shared" si="5"/>
         <v>0.62043795620437958</v>
       </c>
-      <c r="BG31" s="18">
+      <c r="BG31" s="34">
         <f t="shared" si="6"/>
         <v>230.34692100000001</v>
       </c>
@@ -18305,14 +18315,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BEB0B4-AADC-40D3-90FA-3B723F9F987F}">
   <dimension ref="A1:B188"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B194" sqref="B194:B205"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -18324,10 +18336,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="32">
         <v>96.905299999999997</v>
       </c>
     </row>
@@ -18340,10 +18352,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="32">
         <v>94.70805</v>
       </c>
     </row>
@@ -18444,10 +18456,10 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="32">
         <v>16.752949999999998</v>
       </c>
     </row>
@@ -18500,10 +18512,10 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="32">
         <v>4.5026849999999996</v>
       </c>
     </row>
@@ -18676,10 +18688,10 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+      <c r="A48" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="32">
         <v>85</v>
       </c>
     </row>
@@ -18796,10 +18808,10 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>54</v>
-      </c>
-      <c r="B63">
+      <c r="A63" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" s="32">
         <v>138</v>
       </c>
     </row>
@@ -18828,10 +18840,10 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+      <c r="A67" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="32">
         <v>174</v>
       </c>
     </row>
@@ -18868,10 +18880,10 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+      <c r="A72" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="32">
         <v>415</v>
       </c>
     </row>
@@ -18956,18 +18968,18 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+      <c r="A84" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B84" s="20">
+      <c r="B84" s="37">
         <v>0.62043795620437958</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+      <c r="A85" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B85" s="20">
+      <c r="B85" s="37">
         <v>0.62589928057553956</v>
       </c>
     </row>
@@ -19020,10 +19032,10 @@
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+      <c r="A92" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B92" s="20">
+      <c r="B92" s="37">
         <v>0.67424857839155161</v>
       </c>
     </row>
@@ -19132,10 +19144,10 @@
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
-        <v>54</v>
-      </c>
-      <c r="B106" s="20">
+      <c r="A106" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B106" s="37">
         <v>0.83636363636363631</v>
       </c>
     </row>
@@ -19196,10 +19208,10 @@
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
+      <c r="A115" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="32">
         <v>3.1918799999999998</v>
       </c>
     </row>
@@ -19268,10 +19280,10 @@
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
+      <c r="A124" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B124">
+      <c r="B124" s="32">
         <v>1.18963</v>
       </c>
     </row>
@@ -19308,10 +19320,10 @@
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
-        <v>54</v>
-      </c>
-      <c r="B129">
+      <c r="A129" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B129" s="32">
         <v>0.95036600000000004</v>
       </c>
     </row>
@@ -19436,10 +19448,10 @@
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
+      <c r="A145" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B145">
+      <c r="B145" s="32">
         <v>0.35512100000000002</v>
       </c>
     </row>
@@ -19476,18 +19488,18 @@
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A154" t="s">
+      <c r="A154" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B154">
+      <c r="B154" s="32">
         <v>230.34692100000001</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A155" t="s">
-        <v>54</v>
-      </c>
-      <c r="B155">
+      <c r="A155" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B155" s="32">
         <v>218.10341600000001</v>
       </c>
     </row>
@@ -19596,10 +19608,10 @@
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A169" t="s">
+      <c r="A169" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B169">
+      <c r="B169" s="32">
         <v>67.718364999999991</v>
       </c>
     </row>
@@ -19660,10 +19672,10 @@
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A177" t="s">
+      <c r="A177" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B177">
+      <c r="B177" s="32">
         <v>35.295229999999997</v>
       </c>
     </row>

</xml_diff>